<commit_message>
Filtros completos combinados para oficina y secretaria
</commit_message>
<xml_diff>
--- a/docs/FEATURES CAV.xlsx
+++ b/docs/FEATURES CAV.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\cav\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9552" windowHeight="3276"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Reitero de reclamos 1- El mismo con comentarios ( y que quede marcado como reiterado) y agregar comentarios al reclamo. Resaltar el reclamo reiterado para el area</t>
   </si>
@@ -143,17 +138,41 @@
     <t>Que no permita crea vecinos con DNI duplicados, REVISAR SI hacen falta cambios en la DB porque para esto tiene que haber un historial de domicilios.</t>
   </si>
   <si>
-    <t>se pueden subir, falta verlas ( desde el operador )</t>
-  </si>
-  <si>
     <t>Reporte General, dinamico, ( con click de despliegue ) , elegir entre fechas, Total de reclamos por cada secretarias y total por oficina, con sus valores por estados, y separarlos por tipo de reclamo.</t>
+  </si>
+  <si>
+    <t>se pueden subir y verlas ( desde el operador )</t>
+  </si>
+  <si>
+    <t>Copiar Filtros Apellido, DNI, nroReclamo para que lo tenga oficina y secretaria</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Obras Publicas, analizar la posibilidad del hacer el filtro por calle y altura. ( Iniciado - Visto - Conectado )</t>
+  </si>
+  <si>
+    <t>En la ventana de informacion de Vecino falta el domicilio y el horario al que se puede molestar</t>
+  </si>
+  <si>
+    <t>Domicilio de Reclamo se pueda ver con un click y un modal-Ventana. ( Ahora esta el domicilio del reclamante )</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,20 +263,20 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Incorrecto" xfId="3" builtinId="27"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -318,7 +337,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -350,27 +369,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -402,24 +403,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -595,21 +578,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:D34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A4:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="124.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="28.8">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -617,7 +600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -625,7 +608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -633,7 +616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -641,10 +624,10 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -655,12 +638,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="2">
         <v>42874</v>
       </c>
@@ -671,22 +654,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="11" t="s">
+    <row r="12" spans="1:4">
+      <c r="B12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="11"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+    <row r="13" spans="1:4">
+      <c r="B13" s="10"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B14" t="s">
@@ -695,31 +678,31 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
+    <row r="15" spans="1:4">
+      <c r="A15" s="11"/>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="12"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="11"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="12"/>
       <c r="B18" t="s">
         <v>14</v>
@@ -727,30 +710,30 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="12"/>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="12"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="10"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="12"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="10"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4">
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -758,22 +741,22 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>41</v>
+      <c r="B24" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="C24">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+    </row>
+    <row r="26" spans="1:4">
       <c r="B26" t="s">
         <v>20</v>
       </c>
@@ -781,7 +764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -789,12 +772,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4">
       <c r="B28" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -802,7 +785,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -810,7 +793,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
         <v>25</v>
       </c>
@@ -818,22 +801,64 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4">
       <c r="A32" s="8"/>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3">
       <c r="B33" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3">
       <c r="B34" s="4" t="s">
         <v>39</v>
       </c>
     </row>
+    <row r="37" spans="2:3">
+      <c r="C37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C19:C21"/>
     <mergeCell ref="D19:D21"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="D12:D13"/>
@@ -842,11 +867,6 @@
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="A16:A21"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C19:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -854,26 +874,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="3" width="37.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.109375" customWidth="1"/>
     <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5">
       <c r="B2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5">
       <c r="B3" t="s">
         <v>30</v>
       </c>
@@ -887,7 +907,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5">
       <c r="B4" t="s">
         <v>29</v>
       </c>
@@ -898,7 +918,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5">
       <c r="B5" t="s">
         <v>34</v>
       </c>
@@ -912,7 +932,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5">
       <c r="E6" s="8"/>
     </row>
   </sheetData>
@@ -922,12 +942,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
reportes de composicion de Oficina
</commit_message>
<xml_diff>
--- a/docs/FEATURES CAV.xlsx
+++ b/docs/FEATURES CAV.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9552" windowHeight="3276"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9552" windowHeight="3276" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" state="hidden" r:id="rId2"/>
+    <sheet name="Hoja5" sheetId="6" r:id="rId3"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId4"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId5"/>
+    <sheet name="TRAMITES" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="134">
   <si>
     <t>Reitero de reclamos 1- El mismo con comentarios ( y que quede marcado como reiterado) y agregar comentarios al reclamo. Resaltar el reclamo reiterado para el area</t>
   </si>
@@ -84,9 +87,6 @@
     <t>Error cuando genero el reporte , de los revisados no aparece uno. De los dos</t>
   </si>
   <si>
-    <t>Marcar en doblegrey en el ROW que le hice click ( por ejemplo OBVSERVACIONES )</t>
-  </si>
-  <si>
     <t>OPERADOR</t>
   </si>
   <si>
@@ -138,12 +138,6 @@
     <t>Que no permita crea vecinos con DNI duplicados, REVISAR SI hacen falta cambios en la DB porque para esto tiene que haber un historial de domicilios.</t>
   </si>
   <si>
-    <t>Reporte General, dinamico, ( con click de despliegue ) , elegir entre fechas, Total de reclamos por cada secretarias y total por oficina, con sus valores por estados, y separarlos por tipo de reclamo.</t>
-  </si>
-  <si>
-    <t>se pueden subir y verlas ( desde el operador )</t>
-  </si>
-  <si>
     <t>Copiar Filtros Apellido, DNI, nroReclamo para que lo tenga oficina y secretaria</t>
   </si>
   <si>
@@ -166,13 +160,276 @@
   </si>
   <si>
     <t>d</t>
+  </si>
+  <si>
+    <t>Buscar por Barrios? O mostrar por calle y altura agrupados?</t>
+  </si>
+  <si>
+    <t>4 mas</t>
+  </si>
+  <si>
+    <t>a)Incorporar los mismos filtros al perfil supervisor pero con la posibilidad de poder seleccionar “secretaria”, oficina, reclamos, es decir es como un Super Secretario</t>
+  </si>
+  <si>
+    <t>c) Cuando aplicas un filtro que genera un reporte extenso e ingresas a ver alguna observación, el foco se fija en la parte superior de la pantalla perdiendo el orden en que venís controlando.</t>
+  </si>
+  <si>
+    <t>d) Sería más practico que guardes las selecciones de filtrado hasta que vuelvas a cambiar alguna o todas las opciones para no tener que volver a seccionar todo en cada búsqueda.</t>
+  </si>
+  <si>
+    <t>b) También hay que permitirle al supervisor ingresar al menú "Reportes" que tiene el admin ahora</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/2246227/keep-values-selected-after-form-submission</t>
+  </si>
+  <si>
+    <t>Separar Filtro de Secretaria y oficina ( actualizar el filtro de Secretaria de forma dinamica )</t>
+  </si>
+  <si>
+    <t>Que el secretario tambien pueda ver las imágenes de los reclamos</t>
+  </si>
+  <si>
+    <t>Que las oficinas tengan los filtros: Apellido, Desde, Hasta, DNI estado, nro Rec.</t>
+  </si>
+  <si>
+    <t>Que las areas de luminaria y delegaciones ( al menos ) puedan tener la opcion del estado "a Reasignar"</t>
+  </si>
+  <si>
+    <t>Que el supervisor le aparezca la posibilidad de cambiar de tipo de reclamo, ( a los que tengan el estado "a Reasignar"  y a otros tambien ),  por ende el se cambia tambien el responsable</t>
+  </si>
+  <si>
+    <t>Que en el listado principal no se muestre ni Gestionados ni Solucionados</t>
+  </si>
+  <si>
+    <t>solicitado por operadores</t>
+  </si>
+  <si>
+    <t>Ya estaba mas arriba</t>
+  </si>
+  <si>
+    <t>Que se mantenga el encabezado al scrollear</t>
+  </si>
+  <si>
+    <t>TAB en la selección de calles</t>
+  </si>
+  <si>
+    <t>Que indique q tipo de reclamo marcaste, onda que te aparezca grisado o algo asi</t>
+  </si>
+  <si>
+    <t>esto ya esta hecho… sino habria que sacar los filtros por reclamos</t>
+  </si>
+  <si>
+    <t>el TH deberia tener algo como esto     position: fixed;
+    top: 20px;
+    background: white; y despues que dada Width del primer row asignarselo para que quedo oka</t>
+  </si>
+  <si>
+    <t>Reporte General, dinamico, ( con click de despliegue ) , total de reclamos por cada secretarias y total por oficina, con sus valores por estados, y separarlos por tipo de reclamo.</t>
+  </si>
+  <si>
+    <t>Marcar en darkgrey en el ROW que le hice click ( por ejemplo OBVSERVACIONES )</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>Funcionalidades anteriores del 19 de Mayo</t>
+  </si>
+  <si>
+    <t>Ya subido al entorno de testing</t>
+  </si>
+  <si>
+    <t>Hasta aca</t>
+  </si>
+  <si>
+    <t>MAX PRIORIDAD</t>
+  </si>
+  <si>
+    <t>Que los reclamos filtrados puedan exportarse a un Excel.</t>
+  </si>
+  <si>
+    <t>en que reportes… en los tres? Falta separar en los reportes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> el que carga el reclamo de este tipo puede hacer editar sus comentarios </t>
+  </si>
+  <si>
+    <t>Tramites</t>
+  </si>
+  <si>
+    <t>Opciones para crear tramites Customizables</t>
+  </si>
+  <si>
+    <t>Inicio de Tramite</t>
+  </si>
+  <si>
+    <t>Cantidad de Pasos</t>
+  </si>
+  <si>
+    <t>Ingreso de Informacion (textArea)</t>
+  </si>
+  <si>
+    <t>Formularios Relevantes</t>
+  </si>
+  <si>
+    <t>Oficinas Involucradas</t>
+  </si>
+  <si>
+    <t>agrupamiento por Tema</t>
+  </si>
+  <si>
+    <t>limitar horarios de atencion por tipo de tramites</t>
+  </si>
+  <si>
+    <t>Cada Paso</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Subir documentos</t>
+  </si>
+  <si>
+    <t>Texto</t>
+  </si>
+  <si>
+    <t>Bajar documentos</t>
+  </si>
+  <si>
+    <t>Oficina que pertenece</t>
+  </si>
+  <si>
+    <t>Tiempo estimado</t>
+  </si>
+  <si>
+    <t>Emplado</t>
+  </si>
+  <si>
+    <t>id_tramite_asociado</t>
+  </si>
+  <si>
+    <t>id_paso</t>
+  </si>
+  <si>
+    <t>Grupos</t>
+  </si>
+  <si>
+    <t>Elegir Agrupamiento</t>
+  </si>
+  <si>
+    <t>Vecino</t>
+  </si>
+  <si>
+    <t>Comercio</t>
+  </si>
+  <si>
+    <t>Transporte</t>
+  </si>
+  <si>
+    <t>Tramites Sociales</t>
+  </si>
+  <si>
+    <t>Alta Persona</t>
+  </si>
+  <si>
+    <t>Paso 1 que se pueda ver el agrupamiento ( 1ero de dic ) ?=</t>
+  </si>
+  <si>
+    <t>lanus gov .ar</t>
+  </si>
+  <si>
+    <t>SITIO DE REFERENCIA de estilos</t>
+  </si>
+  <si>
+    <t>Paso 2 que se pueda Trabajar desde la oficina</t>
+  </si>
+  <si>
+    <t>Paso 3 Tablero de control</t>
+  </si>
+  <si>
+    <t>que cuando filtro por cualquier cosa me contemple los solucionados tambien, salvo cuando no filtro por nada</t>
+  </si>
+  <si>
+    <t>listado de la hoja5</t>
+  </si>
+  <si>
+    <t>Hola Daniel</t>
+  </si>
+  <si>
+    <t>Podés agregar un reporte en el perfil supervisor con los siguiente datos:</t>
+  </si>
+  <si>
+    <t>Secretaria 1</t>
+  </si>
+  <si>
+    <t>Nombre,  Apellido y Usuario</t>
+  </si>
+  <si>
+    <t>        oficina 1</t>
+  </si>
+  <si>
+    <t>        Nombre,  Apellido y Usuario</t>
+  </si>
+  <si>
+    <t>        Tipo de Reclamo 1</t>
+  </si>
+  <si>
+    <t>        Tipo de Reclamo 2</t>
+  </si>
+  <si>
+    <t>        Tipo de Reclamo 3 </t>
+  </si>
+  <si>
+    <t>        Tipo de Reclamo x</t>
+  </si>
+  <si>
+    <t>    </t>
+  </si>
+  <si>
+    <t>        oficina 2</t>
+  </si>
+  <si>
+    <t>        Tipo de Reclamo 1</t>
+  </si>
+  <si>
+    <t>        Tipo de Reclamo 2</t>
+  </si>
+  <si>
+    <t>        Tipo de Reclamo 3</t>
+  </si>
+  <si>
+    <t>Secretaria 2</t>
+  </si>
+  <si>
+    <t>        Tipo de Reclamo x  </t>
+  </si>
+  <si>
+    <t>      oficina 2</t>
+  </si>
+  <si>
+    <t>Secretaria x</t>
+  </si>
+  <si>
+    <t>        </t>
+  </si>
+  <si>
+    <t>Gracias</t>
+  </si>
+  <si>
+    <t>hay tipos de reclamos que tienen el mismo nombre.. No los puden distiguir las diferentes delegaciones a la hora de reasignarlos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hacer dos arrays </t>
+  </si>
+  <si>
+    <t xml:space="preserve">uno con id de padre Intendecia que triga a todos los secretarios </t>
+  </si>
+  <si>
+    <t>otro con todos los  usuario que traiga los tipo de reclamos y esten agrupados por oficina</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,13 +440,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -209,8 +459,57 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF212121"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,12 +523,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -242,13 +553,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -260,37 +575,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
-    <cellStyle name="Incorrecto" xfId="3" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8"/>
+    <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -579,20 +909,343 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:D41"/>
+  <dimension ref="B1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="123.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5">
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5">
+      <c r="B2" s="10">
+        <v>42923</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="10"/>
+      <c r="C3" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="10"/>
+      <c r="C4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="C5" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="C6" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="C7" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="12"/>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="C11" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="10"/>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="14"/>
+      <c r="C13" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="C16" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" s="22"/>
+      <c r="C20" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="C23" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>75</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="C25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="C26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="C27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="C29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="C32" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="C33" s="23"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="H33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="24"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="24"/>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="B37" s="24"/>
+      <c r="C37" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+    </row>
+    <row r="38" spans="2:8">
+      <c r="B38" s="24"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="24"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="E37:E39"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B34:B39"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="D37:D39"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A4:D59"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="124.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="152.5546875" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:4" ht="28.8">
+    <row r="4" spans="1:4">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,11 +1273,8 @@
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -655,21 +1305,21 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9">
+      <c r="C12" s="20"/>
+      <c r="D12" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="B13" s="10"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="21" t="s">
         <v>9</v>
       </c>
       <c r="B14" t="s">
@@ -679,7 +1329,7 @@
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="11"/>
+      <c r="A15" s="21"/>
       <c r="B15" t="s">
         <v>11</v>
       </c>
@@ -687,23 +1337,23 @@
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="12"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="12"/>
+      <c r="A18" s="24"/>
       <c r="B18" t="s">
         <v>14</v>
       </c>
@@ -711,27 +1361,27 @@
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="12"/>
-      <c r="B19" s="10" t="s">
+      <c r="A19" s="24"/>
+      <c r="B19" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="12"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="12"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="D22" s="8"/>
+      <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
@@ -742,19 +1392,19 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>40</v>
+      <c r="B24" s="22" t="s">
+        <v>67</v>
       </c>
       <c r="C24">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="22"/>
     </row>
     <row r="26" spans="1:4">
       <c r="B26" t="s">
@@ -768,88 +1418,187 @@
       <c r="A27" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="B28" s="7" t="s">
-        <v>27</v>
+      <c r="B28" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" t="s">
         <v>22</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="B30" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="8"/>
+      <c r="A32" s="7"/>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="2:3">
-      <c r="B33" s="4" t="s">
+    <row r="34" spans="2:4">
+      <c r="B34" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
-      <c r="B34" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3">
+    <row r="37" spans="2:4">
       <c r="C37">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="2:3">
+    <row r="38" spans="2:4">
       <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="B39" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3">
-      <c r="B39" t="s">
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C39" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3">
-      <c r="B40" t="s">
-        <v>47</v>
-      </c>
-      <c r="C40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3">
-      <c r="B41" t="s">
+    </row>
+    <row r="42" spans="2:4">
+      <c r="B42" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="C44" t="s">
         <v>48</v>
       </c>
-      <c r="C41" t="s">
+    </row>
+    <row r="45" spans="2:4">
+      <c r="B45" s="5" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4">
+      <c r="B46" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4">
+      <c r="B47" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4">
+      <c r="B48" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="B49" s="8"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="10">
+        <v>42923</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="10"/>
+      <c r="B51" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="10"/>
+      <c r="B52" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="B53" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="B54" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="B55" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="B59" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -868,12 +1617,353 @@
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="A16:A21"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C48" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:D75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="47.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4">
+      <c r="B3" s="17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="18"/>
+      <c r="D8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="18"/>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="18"/>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="18"/>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="18"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="18"/>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" s="17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" s="17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" s="17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" s="17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" s="17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" s="17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2">
+      <c r="B64" s="17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2">
+      <c r="B69" s="17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2">
+      <c r="B71" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72" s="17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75" s="17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E6"/>
   <sheetViews>
@@ -890,50 +1980,50 @@
   <sheetData>
     <row r="2" spans="2:5">
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="2:5">
       <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="2:5">
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
         <v>36</v>
       </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="6" spans="2:5">
-      <c r="E6" s="8"/>
+      <c r="E6" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -941,7 +2031,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
@@ -951,4 +2041,164 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:F30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6">
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="C4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="C10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="C11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="C12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="E13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="E14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="E15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="E16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="E17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="E18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="E19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="E20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="E21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
inicio del modulo de tramites en branch aparte
</commit_message>
<xml_diff>
--- a/docs/FEATURES CAV.xlsx
+++ b/docs/FEATURES CAV.xlsx
@@ -4,22 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9552" windowHeight="3276" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9552" windowHeight="3276" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja4" sheetId="4" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="1" state="hidden" r:id="rId2"/>
-    <sheet name="Hoja5" sheetId="6" r:id="rId3"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId4"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId5"/>
-    <sheet name="TRAMITES" sheetId="5" r:id="rId6"/>
+    <sheet name="requisitos 09_11" sheetId="3" r:id="rId1"/>
+    <sheet name="requisitos anteriores" sheetId="4" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" state="hidden" r:id="rId3"/>
+    <sheet name="Hoja5" sheetId="6" r:id="rId4"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId5"/>
+    <sheet name="TRAMITES_consultas 10_NOV" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="141">
   <si>
     <t>Reitero de reclamos 1- El mismo con comentarios ( y que quede marcado como reiterado) y agregar comentarios al reclamo. Resaltar el reclamo reiterado para el area</t>
   </si>
@@ -254,96 +254,6 @@
     <t xml:space="preserve"> el que carga el reclamo de este tipo puede hacer editar sus comentarios </t>
   </si>
   <si>
-    <t>Tramites</t>
-  </si>
-  <si>
-    <t>Opciones para crear tramites Customizables</t>
-  </si>
-  <si>
-    <t>Inicio de Tramite</t>
-  </si>
-  <si>
-    <t>Cantidad de Pasos</t>
-  </si>
-  <si>
-    <t>Ingreso de Informacion (textArea)</t>
-  </si>
-  <si>
-    <t>Formularios Relevantes</t>
-  </si>
-  <si>
-    <t>Oficinas Involucradas</t>
-  </si>
-  <si>
-    <t>agrupamiento por Tema</t>
-  </si>
-  <si>
-    <t>limitar horarios de atencion por tipo de tramites</t>
-  </si>
-  <si>
-    <t>Cada Paso</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Subir documentos</t>
-  </si>
-  <si>
-    <t>Texto</t>
-  </si>
-  <si>
-    <t>Bajar documentos</t>
-  </si>
-  <si>
-    <t>Oficina que pertenece</t>
-  </si>
-  <si>
-    <t>Tiempo estimado</t>
-  </si>
-  <si>
-    <t>Emplado</t>
-  </si>
-  <si>
-    <t>id_tramite_asociado</t>
-  </si>
-  <si>
-    <t>id_paso</t>
-  </si>
-  <si>
-    <t>Grupos</t>
-  </si>
-  <si>
-    <t>Elegir Agrupamiento</t>
-  </si>
-  <si>
-    <t>Vecino</t>
-  </si>
-  <si>
-    <t>Comercio</t>
-  </si>
-  <si>
-    <t>Transporte</t>
-  </si>
-  <si>
-    <t>Tramites Sociales</t>
-  </si>
-  <si>
-    <t>Alta Persona</t>
-  </si>
-  <si>
-    <t>Paso 1 que se pueda ver el agrupamiento ( 1ero de dic ) ?=</t>
-  </si>
-  <si>
-    <t>lanus gov .ar</t>
-  </si>
-  <si>
-    <t>SITIO DE REFERENCIA de estilos</t>
-  </si>
-  <si>
-    <t>Paso 2 que se pueda Trabajar desde la oficina</t>
-  </si>
-  <si>
-    <t>Paso 3 Tablero de control</t>
-  </si>
-  <si>
     <t>que cuando filtro por cualquier cosa me contemple los solucionados tambien, salvo cuando no filtro por nada</t>
   </si>
   <si>
@@ -423,13 +333,124 @@
   </si>
   <si>
     <t>otro con todos los  usuario que traiga los tipo de reclamos y esten agrupados por oficina</t>
+  </si>
+  <si>
+    <t>hecho pero sin los filtros</t>
+  </si>
+  <si>
+    <t>No se encontro este error, ni con verficiacion correcta ni con incorrecta, el estado del reclamos sigue siendo el CONTACTADO y asi figura en los reportes</t>
+  </si>
+  <si>
+    <t>esto es porque ingresaron sin descripcion solo tienen titulo y es identico, se puede agregar una descripcion en la db o buscar ademas la oficina a la que corresponde?</t>
+  </si>
+  <si>
+    <t>resaltado en verde, falta que se cree la oficina de enlace, para hacer este desarrollo especifico a aesa oficina</t>
+  </si>
+  <si>
+    <t>esto es para la oficina de enlace, hay que crearla</t>
+  </si>
+  <si>
+    <t>Que pueda agregar observaciones , editar comentarios y datos de vecino</t>
+  </si>
+  <si>
+    <t>ver reclamos</t>
+  </si>
+  <si>
+    <t>modificar usuario existente en el administrador que traiga la info del mismo</t>
+  </si>
+  <si>
+    <t>me tienen que dar las descripciones del los puntos - para revisar el tema del reasignado</t>
+  </si>
+  <si>
+    <t>pagina el supervisor traer solo los ultimos 30 dias</t>
+  </si>
+  <si>
+    <t>el filtro de supervisor tiene q actulizar las oficinas y poner solo esas cuando se filtro por secretaria</t>
+  </si>
+  <si>
+    <t>y cuando se elije por oficina que solo quede los tipo de reclamo de oficina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reportes </t>
+  </si>
+  <si>
+    <t>nroReclamo,  nombre direccion y localidad de TODO de a dosmil casos por mes</t>
+  </si>
+  <si>
+    <t>en el Vista de Datos del Reclamante, traer tambien la LOCALIDAD y las entrecalles</t>
+  </si>
+  <si>
+    <t>Filtro seleccionable de tipos de reclamos que traiga la info de los vecinos para que se puedan exportar a Excel</t>
+  </si>
+  <si>
+    <t>desp_tr</t>
+  </si>
+  <si>
+    <t>Es necesario acceder al sitio de tramites desde el CAV reclamos? Boton en el CAV ? La idea es que sean los mismos usuarios</t>
+  </si>
+  <si>
+    <t>Los pasos tienen que tener un listainterdelPAso ( checklist )</t>
+  </si>
+  <si>
+    <t>los pasos van a ser diferentes y especificos para cada tramite</t>
+  </si>
+  <si>
+    <t>El logueo es con los mismos usuarios?</t>
+  </si>
+  <si>
+    <t>se define otro perfil.. Operador de tramite</t>
+  </si>
+  <si>
+    <t>es mejor hacerl el tramite integrado solo diferente la pantalla para el ingreso de los vecinos</t>
+  </si>
+  <si>
+    <t>Estoy haciendo un administrador similar al que existe en el CAV para crear los tipos de reclamos, para crear los tipos de Quien y cuando va a subir los tramites?</t>
+  </si>
+  <si>
+    <t>esto va cambiar un poco por lo que hablamos del check list</t>
+  </si>
+  <si>
+    <t>La nomenclatura de los tramites es univoca? Por lo menos para cada oficina?</t>
+  </si>
+  <si>
+    <t>univoca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿ El vecino que ingresa desde la mesa de entrada es de los que estan en la base de datos? </t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿ Debe ser uno de ellos para iniciar el tramites? Elegirse por DNI o Apellido como lo hacen los que toman los reclamos </t>
+  </si>
+  <si>
+    <t>DNI perfecto</t>
+  </si>
+  <si>
+    <t>Como la url del sitio de tramites es otra a la default, deberia poder definir un VirtualHost para el nuevo modulo. O lo hace andres o me da permisos</t>
+  </si>
+  <si>
+    <t>ni falta ahcer</t>
+  </si>
+  <si>
+    <t>No estoy teniendo acceso a los sitios, ( probar desde casa )</t>
+  </si>
+  <si>
+    <t>En diciembre que dia y que es lo que se espera que tenga que presentar?</t>
+  </si>
+  <si>
+    <t>15 dias de diciembre</t>
+  </si>
+  <si>
+    <t>crear el tramitecomo vecino y verlo como oficinista</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,21 +516,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color rgb="FF212121"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -543,6 +556,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -563,7 +582,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -586,16 +605,16 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -610,6 +629,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -909,10 +931,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:H39"/>
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:H42"/>
   <sheetViews>
     <sheetView topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1088,149 +1201,153 @@
       <c r="B24" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="11" t="s">
         <v>21</v>
       </c>
+      <c r="E24" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="25" spans="2:8">
-      <c r="C25" t="s">
-        <v>107</v>
+      <c r="C25" s="19" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="2:8">
-      <c r="C26" t="s">
-        <v>130</v>
+      <c r="C26" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="2:8">
-      <c r="C27" t="s">
-        <v>108</v>
+      <c r="C27" s="19" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="2:8">
-      <c r="C28" t="s">
+      <c r="C28" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D28">
         <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>18</v>
+        <v>107</v>
       </c>
       <c r="H28">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="2:8">
-      <c r="C29" t="s">
+      <c r="C29" s="11" t="s">
         <v>76</v>
       </c>
+      <c r="E29" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>25</v>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" t="s">
+        <v>17</v>
       </c>
       <c r="H30">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="2:8">
-      <c r="B31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" t="s">
-        <v>17</v>
-      </c>
-      <c r="H31">
-        <v>4</v>
+      <c r="C31" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20">
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="2:8">
-      <c r="C32" s="23" t="s">
-        <v>8</v>
-      </c>
+      <c r="C32" s="23"/>
       <c r="D32" s="20"/>
-      <c r="E32" s="20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8">
-      <c r="C33" s="23"/>
+      <c r="E32" s="20"/>
+      <c r="H32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>13</v>
+      </c>
       <c r="D33" s="20"/>
       <c r="E33" s="20"/>
-      <c r="H33">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8">
-      <c r="B34" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>13</v>
-      </c>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" s="24"/>
+      <c r="C34" s="25"/>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
-    </row>
-    <row r="35" spans="2:8">
+      <c r="G34" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7">
       <c r="B35" s="24"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-    </row>
-    <row r="36" spans="2:8">
+      <c r="C35" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="2:7">
       <c r="B36" s="24"/>
-      <c r="C36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-    </row>
-    <row r="37" spans="2:8">
+      <c r="C36" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+    </row>
+    <row r="37" spans="2:7">
       <c r="B37" s="24"/>
-      <c r="C37" s="23" t="s">
-        <v>15</v>
-      </c>
+      <c r="C37" s="23"/>
       <c r="D37" s="20"/>
       <c r="E37" s="20"/>
     </row>
-    <row r="38" spans="2:8">
+    <row r="38" spans="2:7">
       <c r="B38" s="24"/>
       <c r="C38" s="23"/>
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
     </row>
-    <row r="39" spans="2:8">
-      <c r="B39" s="24"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
+    <row r="42" spans="2:7">
+      <c r="C42" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="E37:E39"/>
+    <mergeCell ref="E36:E38"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
     <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B34:B39"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="D36:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:D59"/>
   <sheetViews>
@@ -1603,11 +1720,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C19:C21"/>
     <mergeCell ref="D19:D21"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="D12:D13"/>
@@ -1616,6 +1728,11 @@
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="A16:A21"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C19:C21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C48" r:id="rId1"/>
@@ -1625,11 +1742,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1639,118 +1756,118 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4">
-      <c r="B3" s="17" t="s">
-        <v>109</v>
+      <c r="B3" s="16" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="17" t="s">
-        <v>110</v>
+      <c r="B5" s="16" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="17" t="s">
-        <v>111</v>
+      <c r="B7" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="D7" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="2:4">
-      <c r="B8" s="18"/>
+      <c r="B8" s="17"/>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="2:4">
-      <c r="B9" s="17" t="s">
-        <v>112</v>
+      <c r="B9" s="16" t="s">
+        <v>82</v>
       </c>
       <c r="D9" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="2:4">
-      <c r="B10" s="18"/>
+      <c r="B10" s="17"/>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="18"/>
+      <c r="B11" s="17"/>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="19" t="s">
-        <v>113</v>
+      <c r="B12" s="18" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="2:4">
-      <c r="B13" s="18"/>
+      <c r="B13" s="17"/>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="17" t="s">
-        <v>114</v>
+      <c r="B14" s="16" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="2:4">
-      <c r="B15" s="17" t="s">
-        <v>115</v>
+      <c r="B15" s="16" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="2:4">
-      <c r="B16" s="17" t="s">
-        <v>116</v>
+      <c r="B16" s="16" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="2:2">
-      <c r="B17" s="17" t="s">
-        <v>117</v>
+      <c r="B17" s="16" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="2:2">
-      <c r="B18" s="17" t="s">
-        <v>118</v>
+      <c r="B18" s="16" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="2:2">
-      <c r="B19" s="17" t="s">
-        <v>119</v>
+      <c r="B19" s="16" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="2:2">
-      <c r="B20" s="18"/>
+      <c r="B20" s="17"/>
     </row>
     <row r="21" spans="2:2">
-      <c r="B21" s="19" t="s">
-        <v>120</v>
+      <c r="B21" s="18" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="2:2">
-      <c r="B22" s="18"/>
+      <c r="B22" s="17"/>
     </row>
     <row r="23" spans="2:2">
-      <c r="B23" s="17" t="s">
-        <v>114</v>
+      <c r="B23" s="16" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="2:2">
-      <c r="B24" s="17" t="s">
-        <v>121</v>
+      <c r="B24" s="16" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="2:2">
-      <c r="B25" s="17" t="s">
-        <v>122</v>
+      <c r="B25" s="16" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="2:2">
-      <c r="B26" s="17" t="s">
-        <v>123</v>
+      <c r="B26" s="16" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="2:2">
-      <c r="B27" s="17" t="s">
-        <v>118</v>
+      <c r="B27" s="16" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="2:2">
@@ -1760,8 +1877,8 @@
       <c r="B29" s="1"/>
     </row>
     <row r="30" spans="2:2">
-      <c r="B30" s="17" t="s">
-        <v>124</v>
+      <c r="B30" s="16" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="2:2">
@@ -1771,8 +1888,8 @@
       <c r="B32" s="1"/>
     </row>
     <row r="33" spans="2:2">
-      <c r="B33" s="17" t="s">
-        <v>112</v>
+      <c r="B33" s="16" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="2:2">
@@ -1785,8 +1902,8 @@
       <c r="B36" s="1"/>
     </row>
     <row r="37" spans="2:2">
-      <c r="B37" s="17" t="s">
-        <v>113</v>
+      <c r="B37" s="16" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="2:2">
@@ -1796,77 +1913,77 @@
       <c r="B39" s="1"/>
     </row>
     <row r="40" spans="2:2">
-      <c r="B40" s="17" t="s">
-        <v>114</v>
+      <c r="B40" s="16" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="2:2">
-      <c r="B41" s="17" t="s">
-        <v>121</v>
+      <c r="B41" s="16" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="2:2">
-      <c r="B42" s="17" t="s">
-        <v>122</v>
+      <c r="B42" s="16" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="2:2">
-      <c r="B43" s="17" t="s">
-        <v>123</v>
+      <c r="B43" s="16" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="2:2">
-      <c r="B44" s="17" t="s">
-        <v>125</v>
+      <c r="B44" s="16" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45" s="1"/>
     </row>
     <row r="46" spans="2:2">
-      <c r="B46" s="17" t="s">
-        <v>126</v>
+      <c r="B46" s="16" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="2:2">
-      <c r="B47" s="17" t="s">
-        <v>114</v>
+      <c r="B47" s="16" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="2:2">
-      <c r="B48" s="17" t="s">
-        <v>121</v>
+      <c r="B48" s="16" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="2:2">
-      <c r="B49" s="17" t="s">
-        <v>122</v>
+      <c r="B49" s="16" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="2:2">
-      <c r="B50" s="17" t="s">
-        <v>123</v>
+      <c r="B50" s="16" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="2:2">
-      <c r="B51" s="17" t="s">
-        <v>118</v>
+      <c r="B51" s="16" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52" s="1"/>
     </row>
     <row r="53" spans="2:2">
-      <c r="B53" s="17" t="s">
-        <v>127</v>
+      <c r="B53" s="16" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="2:2">
       <c r="B54" s="1"/>
     </row>
     <row r="55" spans="2:2">
-      <c r="B55" s="17" t="s">
-        <v>112</v>
+      <c r="B55" s="16" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="2:2">
@@ -1876,74 +1993,74 @@
       <c r="B57" s="1"/>
     </row>
     <row r="58" spans="2:2">
-      <c r="B58" s="17" t="s">
-        <v>113</v>
+      <c r="B58" s="16" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="2:2">
       <c r="B59" s="1"/>
     </row>
     <row r="60" spans="2:2">
-      <c r="B60" s="17" t="s">
-        <v>114</v>
+      <c r="B60" s="16" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="2:2">
-      <c r="B61" s="17" t="s">
-        <v>121</v>
+      <c r="B61" s="16" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="62" spans="2:2">
-      <c r="B62" s="17" t="s">
-        <v>122</v>
+      <c r="B62" s="16" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="63" spans="2:2">
-      <c r="B63" s="17" t="s">
-        <v>123</v>
+      <c r="B63" s="16" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="64" spans="2:2">
-      <c r="B64" s="17" t="s">
-        <v>118</v>
+      <c r="B64" s="16" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="65" spans="2:2">
-      <c r="B65" s="17" t="s">
-        <v>128</v>
+      <c r="B65" s="16" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="2:2">
-      <c r="B66" s="17" t="s">
-        <v>120</v>
+      <c r="B66" s="16" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" s="1"/>
     </row>
     <row r="68" spans="2:2">
-      <c r="B68" s="17" t="s">
-        <v>114</v>
+      <c r="B68" s="16" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="69" spans="2:2">
-      <c r="B69" s="17" t="s">
-        <v>121</v>
+      <c r="B69" s="16" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="70" spans="2:2">
-      <c r="B70" s="17" t="s">
-        <v>122</v>
+      <c r="B70" s="16" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="71" spans="2:2">
-      <c r="B71" s="17" t="s">
-        <v>123</v>
+      <c r="B71" s="16" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="72" spans="2:2">
-      <c r="B72" s="17" t="s">
-        <v>118</v>
+      <c r="B72" s="16" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="2:2">
@@ -1953,8 +2070,8 @@
       <c r="B74" s="1"/>
     </row>
     <row r="75" spans="2:2">
-      <c r="B75" s="17" t="s">
-        <v>129</v>
+      <c r="B75" s="16" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1963,7 +2080,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E6"/>
   <sheetViews>
@@ -2031,171 +2148,105 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:F30"/>
+  <dimension ref="B2:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="131.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6">
-      <c r="B3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="C4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="C5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="C6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="C7" t="s">
-        <v>81</v>
-      </c>
-      <c r="F7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="C8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="C9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="C10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="C11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="C12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6">
-      <c r="E13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="E14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="E15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6">
-      <c r="E16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="E17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="E18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="E19" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="E20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="E21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5">
+    <row r="2" spans="2:4">
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="D3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
       <c r="B25" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5">
-      <c r="B26" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5">
-      <c r="B27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
       <c r="B29" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5">
-      <c r="B30" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edicion de  los tramites
</commit_message>
<xml_diff>
--- a/docs/FEATURES CAV.xlsx
+++ b/docs/FEATURES CAV.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9552" windowHeight="3276" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9552" windowHeight="3276" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="requisitos 09_11" sheetId="3" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Hoja5" sheetId="6" r:id="rId4"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId5"/>
     <sheet name="TRAMITES_consultas 10_NOV" sheetId="7" r:id="rId6"/>
+    <sheet name="Hoja3" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="150">
   <si>
     <t>Reitero de reclamos 1- El mismo con comentarios ( y que quede marcado como reiterado) y agregar comentarios al reclamo. Resaltar el reclamo reiterado para el area</t>
   </si>
@@ -444,6 +445,33 @@
   </si>
   <si>
     <t>crear el tramitecomo vecino y verlo como oficinista</t>
+  </si>
+  <si>
+    <t>a matchear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pasos completados +1 == orden del paso </t>
+  </si>
+  <si>
+    <t>ejemplo de</t>
+  </si>
+  <si>
+    <t>paso 5</t>
+  </si>
+  <si>
+    <t>orden 1</t>
+  </si>
+  <si>
+    <t>cementerio26</t>
+  </si>
+  <si>
+    <t>operador_tr</t>
+  </si>
+  <si>
+    <t>ttr_8</t>
+  </si>
+  <si>
+    <t>tr_9</t>
   </si>
 </sst>
 </file>
@@ -1720,6 +1748,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C19:C21"/>
     <mergeCell ref="D19:D21"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="D12:D13"/>
@@ -1728,11 +1761,6 @@
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="A16:A21"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C19:C21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C48" r:id="rId1"/>
@@ -2152,8 +2180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2252,4 +2280,56 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="2" spans="2:5">
+      <c r="B2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>